<commit_message>
implemented adding rooms and subjects using excel file
also tried to clear form inputs after clicking submit buttons in addingData.jsp, but failed miserably, so commented that part out
</commit_message>
<xml_diff>
--- a/web/excel_template.xlsx
+++ b/web/excel_template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FREEUNI\IV Sem\Software Engineering\Final Project\SmartCampus\web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\Programming\Object Oriented Programming\SmartCampus\web\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -62,12 +62,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Sylfaen"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
       <scheme val="minor"/>
@@ -99,8 +99,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>

</xml_diff>

<commit_message>
fixed lecture remover and updated lectures sxcel template
</commit_message>
<xml_diff>
--- a/web/excel_template.xlsx
+++ b/web/excel_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\Programming\Object Oriented Programming\SmartCampus\web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\Programming\Object Oriented Programming\Final\SmartCampus\web\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>subject_name</t>
   </si>
@@ -32,9 +32,6 @@
     <t>room_name</t>
   </si>
   <si>
-    <t>week_day</t>
-  </si>
-  <si>
     <t>start_time</t>
   </si>
   <si>
@@ -47,9 +44,6 @@
     <t>ოთახის ნომერი</t>
   </si>
   <si>
-    <t>შეიყვანეთ რიცხვი(ორშაბათი: 1, კვირა: 7)</t>
-  </si>
-  <si>
     <t>შეიყვანეთ 24-საათიან ფორმატში (HH:mm)</t>
   </si>
   <si>
@@ -57,6 +51,24 @@
   </si>
   <si>
     <t>მეილის მისამართი</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>შეიყვანეთ yyyy-MM-dd ფორმატში</t>
+  </si>
+  <si>
+    <t>num_weeks</t>
+  </si>
+  <si>
+    <t>კვირების რაოდენობა</t>
+  </si>
+  <si>
+    <t>repetition</t>
+  </si>
+  <si>
+    <t>რამდენ კვირაში ერთხელ განმეორდეს (შეიყვანეთ რიცხვი)</t>
   </si>
 </sst>
 </file>
@@ -437,7 +449,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -446,11 +458,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -465,24 +478,36 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>